<commit_message>
In specdoc: Added references and acknowledgements, Added user documentation, Defined intended audience, Added overview of document, Added Product Overview, Added application perspective, Added product functionality, Edited References, Added folders for figures---figure which describes format of generated schedules. Added use-case diagram figure for admin and general user.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="240" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="75" yWindow="-210" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,10 @@
   </si>
   <si>
     <t>Created specification document for group. Edited specification document. Made 4th set of client questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read IEEE specification document guidelines. Read the chapters named 'Requirements Trap' and 'Specification Trap' in the Pragmmatic Programmer book. Edited specifiction document. Added references and acknowledgements, Added user documentation, Defined intended audience, Added overview of document, Added Product Overview, Added application perspective, Added product functionality, Edited References, Added figure which describes format of generated schedules. Created use-case diagram for admin and general user.
+</t>
   </si>
 </sst>
 </file>
@@ -597,7 +601,7 @@
   <dimension ref="A1:I1988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -665,7 +669,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -863,12 +867,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
+    <row r="18" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>42055</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
+      <c r="G18" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
@@ -14662,6 +14674,1967 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -14689,1967 +16662,6 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added agenda for 2-22-14. Added notes to SRS.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="-210" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="690" yWindow="-180" windowWidth="17850" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14674,1967 +14674,6 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -16662,6 +14701,1967 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Specdoc: Updated section 3 to reflect that of IEEE Std 830-1998 standard. Updated font size and font type. Updated Table of Contents. Updated definitions, acronym, abbreviations. Added multiple folders for different submission versions of specdoc to client.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,14 @@
   </si>
   <si>
     <t>Updated minutes. Added client meeting minutes. Added Java language proposal. Read "Don't Make Me Think" front end designers guide. Updated folder structure. Put all client meeting questions in a single folder for team to access/reference them.</t>
+  </si>
+  <si>
+    <t>Team meeting at 1:00pm. Worked on specification document.</t>
+  </si>
+  <si>
+    <t>Worked on specification document. Read IEEE Std 830-1998 document. Formatted functional requirements based on user class (A3 template format). Updated section 3 to reflect that of IEEE Std 830-1998 standard.
+Updated font size and font type to be more consistent throughout document.
+Updated Table of Contents to reflect contents of document. Added multiple folders for submission versions of specdoc to client.</t>
   </si>
 </sst>
 </file>
@@ -609,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -678,7 +686,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -937,18 +945,34 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
+      <c r="A22" s="6">
+        <v>42062</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
+      <c r="G22" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42063</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
+      <c r="G23" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
@@ -14707,1967 +14731,6 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -16695,6 +14758,1967 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added dates to specdoc version. Updated jeffrey worklog.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>47</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="7">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -14731,6 +14731,1967 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -14758,1967 +16719,6 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated specdoc 1.4. Added meeting minutes for 3-2-2015. Added initial draft of specdoc for references.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="-180" windowWidth="17850" windowHeight="8610"/>
+    <workbookView xWindow="690" yWindow="-180" windowWidth="17850" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -91,6 +91,12 @@
     <t>Worked on specification document. Read IEEE Std 830-1998 document. Formatted functional requirements based on user class (A3 template format). Updated section 3 to reflect that of IEEE Std 830-1998 standard.
 Updated font size and font type to be more consistent throughout document.
 Updated Table of Contents to reflect contents of document. Added multiple folders for submission versions of specdoc to client.</t>
+  </si>
+  <si>
+    <t>2/29/2015</t>
+  </si>
+  <si>
+    <t>Went through Java Scene Builder tutorial. Added standard format to input file. Cleaned document format. Reread specifications requirements chapter in text book for class.</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
   <dimension ref="A1:I1988"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -686,7 +692,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>47.5</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,12 +980,20 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
+    <row r="24" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
+      <c r="G24" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
@@ -14731,1967 +14745,6 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -16719,6 +14772,1967 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated specdoc 1.4. Updated dictionary. Added a date to Deliverables section.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -93,10 +93,16 @@
 Updated Table of Contents to reflect contents of document. Added multiple folders for submission versions of specdoc to client.</t>
   </si>
   <si>
-    <t>2/29/2015</t>
+    <t>Went through Java Scene Builder tutorial. Added standard format to input file. Cleaned document format. Reread specifications requirements chapter in text book for class.</t>
   </si>
   <si>
-    <t>Went through Java Scene Builder tutorial. Added standard format to input file. Cleaned document format. Reread specifications requirements chapter in text book for class.</t>
+    <t>Updated specdoc 1.4. Added meeting agenda for next meeting. Added first ever draft of specdoc for references.</t>
+  </si>
+  <si>
+    <t>Updated meeting minutes. Updated client questions/answers. Merge fix on git.</t>
+  </si>
+  <si>
+    <t>Read coding standards worksheet. Added time constraint figure. Added draft of programming language proposal. Updated "answers to questions". Edited/updated specdoc.</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -692,7 +698,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>49.5</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -981,11 +987,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>24</v>
+      <c r="A24" s="6">
+        <v>42064</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -995,26 +1001,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42065</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="A26" s="6">
+        <v>42066</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
+      <c r="G26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>42068</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
+      <c r="G27" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
@@ -14745,6 +14775,1967 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -14772,1967 +16763,6 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated jeffreys worklog. Moved ResearchDocs to Documents/ResearchDocs
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -112,6 +112,9 @@
   <si>
     <t xml:space="preserve">Team meeting. Updated specdoc sections 2.2 and 2.3. Uploaded Jordan's test files. Collaborated with Riley on coding standards. Updated definitions, acronym, abbreviations in specdoc. Added Screenshots for Version 1 and 2. Updated fonts. Updated references in document to match figures in appendix.
 </t>
+  </si>
+  <si>
+    <t>Went through C# tutorial. Made first C# GUI project. Communicated with Jordan and uploaded his C++ program that generated test files.</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
   <dimension ref="A1:I1988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -707,7 +710,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>59.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1">
@@ -1055,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="74" customHeight="1">
+    <row r="28" spans="1:7" ht="78" customHeight="1">
       <c r="A28" s="6">
         <v>42069</v>
       </c>
@@ -1070,12 +1073,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="B29" s="11"/>
+    <row r="29" spans="1:7" ht="31" customHeight="1">
+      <c r="A29" s="6">
+        <v>42070</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
+      <c r="G29" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="11"/>
@@ -14792,6 +14803,1967 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -14819,1967 +16791,6 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added meeting minutes for 4-16.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="540" yWindow="-345" windowWidth="19950" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Researched transition screens for C#. Reviewed C# tutorial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fixed date on one of the meeting minute folders</t>
+  </si>
+  <si>
+    <t>Fixed some meeting dates, fixed date on minutes. Printed documents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Added maxbinaryheap in c#. Began working on scheduling algorithm. Added meeting minutes 4-7. Worked in Jeffrey's Sandbox: finished priority queue in C#. Worked with Scott and Josh on scheduling algorithm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created class diagrams for class/class list/compressed class list. </t>
+  </si>
+  <si>
+    <t>Researched Welsh-Powell algorithm. Researched</t>
   </si>
 </sst>
 </file>
@@ -393,6 +408,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -415,15 +439,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -729,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -746,35 +761,35 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="8" t="s">
         <v>2</v>
       </c>
@@ -786,19 +801,19 @@
       <c r="A4" s="5">
         <v>42025</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="9">
         <v>2.5</v>
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>98</v>
+        <v>100.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1285,13 +1300,13 @@
       <c r="A37" s="6">
         <v>42086</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="7">
         <v>1</v>
       </c>
@@ -1386,36 +1401,70 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
+    <row r="44" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>42095</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
+      <c r="G44" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
+      <c r="A45" s="6">
+        <v>42096</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
+      <c r="G45" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>42101</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
+      <c r="G46" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
+      <c r="A47" s="6">
+        <v>42102</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
+      <c r="A48" s="6">
+        <v>42103</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -15003,1967 +15052,6 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -16991,6 +15079,1967 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated User Manual. Updated meeting minutes for 4-23. Updated work log.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/jeffrey_worklog.xlsx
+++ b/Documents/WorkLogs/jeffrey_worklog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -171,7 +171,16 @@
     <t xml:space="preserve">Created class diagrams for class/class list/compressed class list. </t>
   </si>
   <si>
-    <t>Researched Welsh-Powell algorithm. Researched</t>
+    <t>Researched acedemic papers on Time Table Scheduling. Researched Welsh-Powell algorithm.</t>
+  </si>
+  <si>
+    <t>Discussed research papers on scheduling algorithms with Scott and Josh. Worked with Josh on reviewing acedemic papers on Time Scheduling algorithms, using graph coloring.</t>
+  </si>
+  <si>
+    <t>Implemented matrix library into personal sandbox folder for scheduler. Updated user's manual. Version 1 and Version 2.</t>
+  </si>
+  <si>
+    <t>Worked on user manual. Added screenshots for login screens. Researched user manual's of various commercial products (Service manuals)</t>
   </si>
 </sst>
 </file>
@@ -744,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:F45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -813,7 +822,7 @@
       </c>
       <c r="I4" s="1">
         <f>SUM(G4:G1993)</f>
-        <v>100.25</v>
+        <v>109.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,8 +1466,11 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>42103</v>
       </c>
@@ -1469,113 +1481,137 @@
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
+      <c r="G48" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>42104</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
+      <c r="G49" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>42105</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
+      <c r="G50" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>42107</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -15052,6 +15088,1967 @@
     </row>
   </sheetData>
   <mergeCells count="1988">
+    <mergeCell ref="B1986:F1986"/>
+    <mergeCell ref="B1987:F1987"/>
+    <mergeCell ref="B1988:F1988"/>
+    <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1981:F1981"/>
+    <mergeCell ref="B1982:F1982"/>
+    <mergeCell ref="B1983:F1983"/>
+    <mergeCell ref="B1984:F1984"/>
+    <mergeCell ref="B1985:F1985"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1975:F1975"/>
+    <mergeCell ref="B1976:F1976"/>
+    <mergeCell ref="B1977:F1977"/>
+    <mergeCell ref="B1978:F1978"/>
+    <mergeCell ref="B1979:F1979"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
@@ -15079,1967 +17076,6 @@
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1986:F1986"/>
-    <mergeCell ref="B1987:F1987"/>
-    <mergeCell ref="B1988:F1988"/>
-    <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1981:F1981"/>
-    <mergeCell ref="B1982:F1982"/>
-    <mergeCell ref="B1983:F1983"/>
-    <mergeCell ref="B1984:F1984"/>
-    <mergeCell ref="B1985:F1985"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1975:F1975"/>
-    <mergeCell ref="B1976:F1976"/>
-    <mergeCell ref="B1977:F1977"/>
-    <mergeCell ref="B1978:F1978"/>
-    <mergeCell ref="B1979:F1979"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>